<commit_message>
update for CalPERS draft
</commit_message>
<xml_diff>
--- a/inputs/data_raw/Data_CalPERS_planInfo_AV2018.xlsx
+++ b/inputs/data_raw/Data_CalPERS_planInfo_AV2018.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Proj_CAPlans\model_CalPERS\inputs\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6E98B8-ACC4-4610-B90E-854DF75E198F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92C7796-62FB-41E2-9FCF-35899EA911CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="18240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -789,7 +789,7 @@
     <numFmt numFmtId="167" formatCode="0.000%"/>
     <numFmt numFmtId="168" formatCode="\$#,##0_);\(\$#,##0\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1777,17 +1777,17 @@
       <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>20180630</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="C6" t="s">
         <v>1</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="C7">
         <v>2019</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="C8">
         <v>2020</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="C9">
         <v>2021</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="C10">
         <v>2022</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="D11" s="2"/>
     </row>
   </sheetData>
@@ -1866,11 +1866,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FFFA73-2D4A-4AA3-8BAA-C57267D0CB48}">
   <dimension ref="A1:M109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="Q86" sqref="Q86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
@@ -1883,7 +1883,7 @@
     <col min="11" max="12" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1893,7 +1893,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="87"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1906,7 +1906,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="87"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="87"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1932,14 +1932,14 @@
       <c r="F4" s="6"/>
       <c r="G4" s="87"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13">
       <c r="C5" s="4"/>
       <c r="D5" s="2"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6"/>
       <c r="G5" s="87"/>
     </row>
-    <row r="6" spans="1:13" s="4" customFormat="1" ht="36" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" s="4" customFormat="1" ht="36">
       <c r="C6" s="7"/>
       <c r="D6" s="34" t="s">
         <v>8</v>
@@ -1963,7 +1963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.5" customHeight="1">
       <c r="C7" t="s">
         <v>71</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="13.5" customHeight="1">
       <c r="C8" t="s">
         <v>75</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="13.5" customHeight="1">
       <c r="C9" t="s">
         <v>75</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13.5" customHeight="1">
       <c r="C10" t="s">
         <v>75</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.5" customHeight="1">
       <c r="C11" t="s">
         <v>75</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13.5" customHeight="1">
       <c r="C12" t="s">
         <v>75</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="13.5" customHeight="1">
       <c r="C13" t="s">
         <v>75</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="13.5" customHeight="1">
       <c r="C14" t="s">
         <v>75</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="13.5" customHeight="1">
       <c r="C15" t="s">
         <v>75</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="13.5" customHeight="1">
       <c r="C16" t="s">
         <v>75</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" ht="13.5" customHeight="1">
       <c r="C17" t="s">
         <v>75</v>
       </c>
@@ -2348,7 +2348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" ht="13.5" customHeight="1">
       <c r="C18" t="s">
         <v>75</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" ht="13.5" customHeight="1">
       <c r="C19" t="s">
         <v>75</v>
       </c>
@@ -2418,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:13" ht="13.5" customHeight="1">
       <c r="C20" t="s">
         <v>75</v>
       </c>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:13" ht="13.5" customHeight="1">
       <c r="C21" t="s">
         <v>75</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" ht="13.5" customHeight="1">
       <c r="C22" t="s">
         <v>75</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" ht="13.5" customHeight="1">
       <c r="C23" t="s">
         <v>75</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" ht="13.5" customHeight="1">
       <c r="C24" t="s">
         <v>75</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" ht="13.5" customHeight="1">
       <c r="C25" t="s">
         <v>75</v>
       </c>
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" ht="13.5" customHeight="1">
       <c r="C26" t="s">
         <v>75</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" ht="13.5" customHeight="1">
       <c r="C27" t="s">
         <v>75</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" ht="13.5" customHeight="1">
       <c r="C28" t="s">
         <v>75</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" ht="13.5" customHeight="1">
       <c r="C29" t="s">
         <v>76</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13">
       <c r="C30" t="s">
         <v>76</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:13">
       <c r="C31" t="s">
         <v>76</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:13">
       <c r="C32" t="s">
         <v>76</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:13">
       <c r="C33" t="s">
         <v>76</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:13">
       <c r="C34" t="s">
         <v>76</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:13" ht="24" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:13" ht="24">
       <c r="C35" t="s">
         <v>76</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:13" ht="24" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:13" ht="24">
       <c r="C36" t="s">
         <v>76</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:13">
       <c r="C37" t="s">
         <v>76</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:13">
       <c r="C38" t="s">
         <v>76</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:13">
       <c r="C39" t="s">
         <v>76</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:13">
       <c r="C40" t="s">
         <v>76</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:13">
       <c r="C41" t="s">
         <v>76</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:13">
       <c r="C42" t="s">
         <v>76</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:13">
       <c r="C43" t="s">
         <v>76</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:13">
       <c r="C44" t="s">
         <v>76</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:13">
       <c r="C45" t="s">
         <v>76</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:13">
       <c r="C46" t="s">
         <v>76</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:13">
       <c r="C47" t="s">
         <v>76</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:13">
       <c r="C48" t="s">
         <v>77</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:13">
       <c r="C49" t="s">
         <v>77</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:13">
       <c r="C50" t="s">
         <v>77</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:13">
       <c r="C51" t="s">
         <v>77</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:13">
       <c r="C52" t="s">
         <v>77</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:13">
       <c r="C53" t="s">
         <v>77</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:13" ht="24" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:13" ht="24">
       <c r="C54" t="s">
         <v>77</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:13" ht="24">
       <c r="C55" t="s">
         <v>77</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:13">
       <c r="C56" t="s">
         <v>77</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:13">
       <c r="C57" t="s">
         <v>77</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:13">
       <c r="C58" t="s">
         <v>77</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:13">
       <c r="C59" t="s">
         <v>77</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:13">
       <c r="C60" t="s">
         <v>77</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:13">
       <c r="C61" t="s">
         <v>77</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:13">
       <c r="C62" t="s">
         <v>77</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:13">
       <c r="C63" t="s">
         <v>77</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:13">
       <c r="C64" t="s">
         <v>77</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:13">
       <c r="C65" t="s">
         <v>77</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:13">
       <c r="C66" t="s">
         <v>77</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:13" ht="15" customHeight="1">
       <c r="C67" t="s">
         <v>78</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:13" ht="15" customHeight="1">
       <c r="C68" t="s">
         <v>78</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:13" ht="15" customHeight="1">
       <c r="C69" t="s">
         <v>78</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:13" ht="15" customHeight="1">
       <c r="C70" t="s">
         <v>78</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:13" ht="15" customHeight="1">
       <c r="C71" t="s">
         <v>78</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:13" ht="15" customHeight="1">
       <c r="C72" t="s">
         <v>78</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:13" ht="15" customHeight="1">
       <c r="C73" t="s">
         <v>78</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="3:13" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:13" ht="24" customHeight="1">
       <c r="C74" t="s">
         <v>78</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:13" ht="15" customHeight="1">
       <c r="C75" t="s">
         <v>78</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:13" ht="15" customHeight="1">
       <c r="C76" t="s">
         <v>78</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:13" ht="15" customHeight="1">
       <c r="C77" t="s">
         <v>78</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:13" ht="15" customHeight="1">
       <c r="C78" t="s">
         <v>78</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:13" ht="15" customHeight="1">
       <c r="C79" t="s">
         <v>78</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:13" ht="15" customHeight="1">
       <c r="C80" t="s">
         <v>78</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:13" ht="15" customHeight="1">
       <c r="C81" t="s">
         <v>78</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:13" ht="15" customHeight="1">
       <c r="C82" t="s">
         <v>78</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:13" ht="15" customHeight="1">
       <c r="C83" t="s">
         <v>78</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:13" ht="15" customHeight="1">
       <c r="C84" t="s">
         <v>78</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:13" ht="15" customHeight="1">
       <c r="C85" t="s">
         <v>78</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:13" ht="15" customHeight="1">
       <c r="C86" t="s">
         <v>78</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="3:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:13" ht="15" customHeight="1">
       <c r="C87" t="s">
         <v>79</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:13">
       <c r="C88" t="s">
         <v>79</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:13">
       <c r="C89" t="s">
         <v>79</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:13">
       <c r="C90" t="s">
         <v>79</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:13">
       <c r="C91" t="s">
         <v>79</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:13" ht="24">
       <c r="C92" t="s">
         <v>79</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:13" ht="24">
       <c r="C93" t="s">
         <v>79</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="3:13" ht="24" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:13" ht="24">
       <c r="C94" t="s">
         <v>79</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:13" ht="24">
       <c r="C95" t="s">
         <v>79</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:13" ht="24">
       <c r="C96" t="s">
         <v>79</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:13" ht="24">
       <c r="C97" t="s">
         <v>79</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:13" ht="24">
       <c r="C98" t="s">
         <v>79</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:13">
       <c r="C99" t="s">
         <v>79</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:13">
       <c r="C100" t="s">
         <v>79</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:13">
       <c r="C101" t="s">
         <v>79</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:13">
       <c r="C102" t="s">
         <v>79</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:13">
       <c r="C103" t="s">
         <v>79</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:13">
       <c r="C104" t="s">
         <v>79</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:13">
       <c r="C105" t="s">
         <v>79</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:13">
       <c r="C106" t="s">
         <v>79</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:13">
       <c r="C107" t="s">
         <v>79</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:13">
       <c r="C108" t="s">
         <v>79</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:13">
       <c r="C109" t="s">
         <v>79</v>
       </c>
@@ -5585,7 +5585,7 @@
       <selection activeCell="B4" sqref="B4:I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
@@ -5595,7 +5595,7 @@
     <col min="10" max="10" width="15.42578125" style="74" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" ht="36" customHeight="1">
       <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -5648,7 +5648,7 @@
       </c>
       <c r="J4" s="11"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10">
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>8.4399999999999996E-3</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>1.618E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10">
       <c r="B7" t="s">
         <v>75</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>1.2409999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10">
       <c r="B8" t="s">
         <v>75</v>
       </c>
@@ -5764,7 +5764,7 @@
         <v>3.7740000000000003E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10">
       <c r="B9" t="s">
         <v>75</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>4.5799999999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10">
       <c r="B10" t="s">
         <v>75</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>1.4499999999999999E-3</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="24">
       <c r="B11" t="s">
         <v>75</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" ht="24">
       <c r="B12" t="s">
         <v>75</v>
       </c>
@@ -5880,7 +5880,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" ht="24">
       <c r="B13" t="s">
         <v>75</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" ht="24">
       <c r="B14" t="s">
         <v>75</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" ht="24">
       <c r="B15" t="s">
         <v>75</v>
       </c>
@@ -5967,7 +5967,7 @@
         <v>7.2679999999999995E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10">
       <c r="B16" t="s">
         <v>75</v>
       </c>
@@ -5996,7 +5996,7 @@
         <v>6.3699999999999998E-3</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10">
       <c r="B17" t="s">
         <v>75</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10">
       <c r="B18" t="s">
         <v>75</v>
       </c>
@@ -6054,7 +6054,7 @@
         <v>1.2E-4</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10">
       <c r="B19" t="s">
         <v>75</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>1.58E-3</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10">
       <c r="B20" t="s">
         <v>75</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>1.8500000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10">
       <c r="B21" t="s">
         <v>75</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>2.477E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10">
       <c r="B22" t="s">
         <v>75</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>1.636E-2</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10">
       <c r="B23" t="s">
         <v>75</v>
       </c>
@@ -6199,7 +6199,7 @@
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10">
       <c r="B24" t="s">
         <v>75</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:10">
       <c r="B25" t="s">
         <v>75</v>
       </c>
@@ -6257,7 +6257,7 @@
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:10">
       <c r="B26" t="s">
         <v>75</v>
       </c>
@@ -6295,7 +6295,7 @@
       <selection activeCell="B4" sqref="B4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="6" width="11.42578125" customWidth="1"/>
@@ -6303,7 +6303,7 @@
     <col min="8" max="9" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="98" t="s">
         <v>35</v>
       </c>
@@ -6316,7 +6316,7 @@
       <c r="I3" s="98"/>
       <c r="J3" s="98"/>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="60">
       <c r="B4" s="34" t="s">
         <v>8</v>
       </c>
@@ -6343,7 +6343,7 @@
       </c>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -6371,7 +6371,7 @@
       <c r="I5" s="11"/>
       <c r="J5" s="41"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -6401,7 +6401,7 @@
       </c>
       <c r="J6" s="41"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -6431,7 +6431,7 @@
       </c>
       <c r="J7" s="41"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -6461,7 +6461,7 @@
       </c>
       <c r="J8" s="41"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="J9" s="41"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="J10" s="41"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>76</v>
       </c>
@@ -6551,7 +6551,7 @@
       </c>
       <c r="J11" s="41"/>
     </row>
-    <row r="12" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="24">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -6581,7 +6581,7 @@
       </c>
       <c r="J12" s="41"/>
     </row>
-    <row r="13" spans="1:10" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="24">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -6611,7 +6611,7 @@
       </c>
       <c r="J13" s="41"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -6641,7 +6641,7 @@
       </c>
       <c r="J14" s="41"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -6671,7 +6671,7 @@
       </c>
       <c r="J15" s="41"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -6701,7 +6701,7 @@
       </c>
       <c r="J16" s="41"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -6731,7 +6731,7 @@
       </c>
       <c r="J17" s="41"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -6761,7 +6761,7 @@
       </c>
       <c r="J18" s="41"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>76</v>
       </c>
@@ -6791,7 +6791,7 @@
       </c>
       <c r="J19" s="41"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -6821,7 +6821,7 @@
       </c>
       <c r="J20" s="41"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -6851,7 +6851,7 @@
       </c>
       <c r="J21" s="41"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -6881,7 +6881,7 @@
       </c>
       <c r="J22" s="41"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>76</v>
       </c>
@@ -6911,7 +6911,7 @@
       </c>
       <c r="J23" s="41"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -6941,7 +6941,7 @@
       </c>
       <c r="J24" s="41"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>76</v>
       </c>
@@ -6985,13 +6985,13 @@
       <selection activeCell="A6" sqref="A6:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="9" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="B3" s="101" t="s">
         <v>48</v>
       </c>
@@ -7003,7 +7003,7 @@
       <c r="H3" s="55"/>
       <c r="I3" s="56"/>
     </row>
-    <row r="4" spans="1:9" ht="84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="84">
       <c r="B4" s="34" t="s">
         <v>8</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -7056,7 +7056,7 @@
       </c>
       <c r="I5" s="11"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>77</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>1.0959999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>6.6100000000000004E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>1.9550000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>2.8800000000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>77</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>3.15E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="24">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -7259,7 +7259,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -7288,7 +7288,7 @@
         <v>5.7600000000000004E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -7317,7 +7317,7 @@
         <v>4.3800000000000002E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -7375,7 +7375,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>2.2280000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -7433,7 +7433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>5.1599999999999997E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -7491,7 +7491,7 @@
         <v>1.0030000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>7.4200000000000004E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -7607,7 +7607,7 @@
         <v>1.14E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -7648,14 +7648,14 @@
       <selection activeCell="A7" sqref="A7:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="9" width="14.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="B3" s="82" t="s">
         <v>49</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
     </row>
-    <row r="4" spans="1:14" ht="48" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="48">
       <c r="B4" s="34" t="s">
         <v>8</v>
       </c>
@@ -7695,7 +7695,7 @@
       </c>
       <c r="J4" s="41"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="B5" s="76"/>
       <c r="C5" s="77"/>
       <c r="D5" s="40"/>
@@ -7706,7 +7706,7 @@
       <c r="I5" s="79"/>
       <c r="J5" s="41"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -7734,7 +7734,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="41"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -7773,7 +7773,7 @@
         <v>45827301</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="15" customHeight="1">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>69481771</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="15" customHeight="1">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>68070175</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v>224300335</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="15" customHeight="1">
       <c r="A11" t="s">
         <v>78</v>
       </c>
@@ -7929,7 +7929,7 @@
         <v>5652570</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>78</v>
       </c>
@@ -7968,7 +7968,7 @@
         <v>28975135</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>78</v>
       </c>
@@ -8007,7 +8007,7 @@
         <v>31397747</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" customHeight="1">
       <c r="A14" t="s">
         <v>78</v>
       </c>
@@ -8046,7 +8046,7 @@
         <v>-6671056</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>78</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>2176996</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="15" customHeight="1">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -8124,7 +8124,7 @@
         <v>26701683</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15" customHeight="1">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -8163,7 +8163,7 @@
         <v>3086595</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15" customHeight="1">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -8202,7 +8202,7 @@
         <v>20325926</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15" customHeight="1">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>302704781</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="15" customHeight="1">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>-167613</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="15" customHeight="1">
       <c r="A21" t="s">
         <v>78</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>109658226</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15" customHeight="1">
       <c r="A22" t="s">
         <v>78</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>84733104</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15" customHeight="1">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -8397,7 +8397,7 @@
         <v>72378064</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="15" customHeight="1">
       <c r="A24" t="s">
         <v>78</v>
       </c>
@@ -8436,7 +8436,7 @@
         <v>-24691671</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15" customHeight="1">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>-2552870</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="15" customHeight="1">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -8514,7 +8514,7 @@
         <v>8198945</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -8536,7 +8536,7 @@
       </c>
       <c r="J27" s="41"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>78</v>
       </c>
@@ -8569,7 +8569,7 @@
       <selection activeCell="A7" sqref="A7:H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="9" width="16.28515625" customWidth="1"/>
@@ -8578,7 +8578,7 @@
     <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="B3" s="101" t="s">
         <v>66</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="H3" s="106"/>
       <c r="I3" s="59"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="B4" s="102"/>
       <c r="C4" s="103"/>
       <c r="D4" s="105"/>
@@ -8609,7 +8609,7 @@
         <v>7527113</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="48">
       <c r="B5" s="34" t="s">
         <v>8</v>
       </c>
@@ -8635,7 +8635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>71</v>
       </c>
@@ -8665,7 +8665,7 @@
       <c r="M6" s="109"/>
       <c r="N6" s="109"/>
     </row>
-    <row r="7" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -8694,7 +8694,7 @@
         <v>8.1799999999999998E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -8723,7 +8723,7 @@
         <v>1.8450000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -8752,7 +8752,7 @@
         <v>1.917E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -8781,7 +8781,7 @@
         <v>8.6629999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -8810,7 +8810,7 @@
         <v>8.6499999999999997E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -8839,7 +8839,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>79</v>
       </c>
@@ -8868,7 +8868,7 @@
         <v>2.155E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -8926,7 +8926,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>2.7999999999999998E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -8984,7 +8984,7 @@
         <v>4.2000000000000002E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -9013,7 +9013,7 @@
         <v>0.12870000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -9042,7 +9042,7 @@
         <v>2.3480000000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
         <v>79</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>7.6299999999999996E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>1.541E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -9158,7 +9158,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>3.4419999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -9216,7 +9216,7 @@
         <v>3.1119999999999998E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -9245,7 +9245,7 @@
         <v>1.503E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
         <v>79</v>
       </c>
@@ -9274,7 +9274,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -9303,7 +9303,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -9332,7 +9332,7 @@
         <v>2.1299999999999999E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9">
       <c r="B30" s="31" t="s">
         <v>34</v>
       </c>

</xml_diff>